<commit_message>
v1.2 Review Status Closed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_DELETEPOST_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_DELETEPOST_REVIEWS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CFF0F8-F34D-4ED3-A224-EBE232FCAADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_WF_DELETEPOST_REVIEW" sheetId="3" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -62,9 +63,6 @@
   </si>
   <si>
     <t>v1.0</t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t>Omar Sherif</t>
@@ -114,17 +112,20 @@
     <t>v1.1</t>
   </si>
   <si>
-    <t>emna</t>
-  </si>
-  <si>
     <t>update owner status</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>Review Status closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,35 +610,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" ht="37.5">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -666,94 +667,94 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="90">
+    <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>23</v>
-      </c>
       <c r="G2" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="105">
-      <c r="A3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="G3" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="60">
-      <c r="A4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="I4" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -764,7 +765,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -775,7 +776,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -786,7 +787,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -797,7 +798,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -808,7 +809,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -819,7 +820,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -830,7 +831,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -844,10 +845,10 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I4:I12 I2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I4:I12 I2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -856,22 +857,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25">
+    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -885,37 +886,47 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.5">
+    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="7">
         <v>45776</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75">
+    <row r="3" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="7">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7">
+        <v>45806</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>